<commit_message>
Added Add Customer Test script
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="5520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
     <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -399,7 +400,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -457,7 +458,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>